<commit_message>
First ready to deploy Network ARM template
</commit_message>
<xml_diff>
--- a/TemplatesARM/ResourcesForARM.xlsx
+++ b/TemplatesARM/ResourcesForARM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TemplatesARM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\TemplatesARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{324A8B97-DBDF-456C-82B8-6C05BA8CB1D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AC5256-2100-442B-A817-30C7AF7AE88C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{B9E6AA66-0A81-4F7C-AAC2-58304DAA1CCE}"/>
   </bookViews>
@@ -30,14 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ResourceGroup</t>
   </si>
   <si>
-    <t>Network</t>
-  </si>
-  <si>
     <t>Subnet1</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>NIC1-2</t>
   </si>
   <si>
-    <t>AvSet1</t>
-  </si>
-  <si>
     <t>PublicIP1</t>
   </si>
   <si>
@@ -90,6 +84,27 @@
   </si>
   <si>
     <t>LB2NATRDP</t>
+  </si>
+  <si>
+    <t>ARM Network</t>
+  </si>
+  <si>
+    <t>ARM VM</t>
+  </si>
+  <si>
+    <t>ARM LB</t>
+  </si>
+  <si>
+    <t>AvSet</t>
+  </si>
+  <si>
+    <t>Network1</t>
+  </si>
+  <si>
+    <t>Network2</t>
+  </si>
+  <si>
+    <t>PSScript</t>
   </si>
 </sst>
 </file>
@@ -113,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -121,15 +136,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,110 +480,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737AB9F4-C28E-49D6-911F-D614C71E9380}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.109375" customWidth="1"/>
     <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C2:C4"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C5:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>